<commit_message>
Add week 12 content
</commit_message>
<xml_diff>
--- a/docsrc/source/_static/Examples/DCF/Forecasting/Simple/Sales COGS Forecasted.xlsx
+++ b/docsrc/source/_static/Examples/DCF/Forecasting/Simple/Sales COGS Forecasted.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UF\Teaching\Modeling\Me\repos\fin-model-course\Examples\DCF\Forecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71B7588-6E61-4142-9349-8B8EE40B8418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A20CC875-FFB2-4171-B6DD-F0E8E9B4C378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29520" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{B3DEEA20-6275-4550-BD4B-1C18D7A950FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3DEEA20-6275-4550-BD4B-1C18D7A950FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$H$7:$W$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$7:$W$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>Sales</t>
   </si>
@@ -73,16 +75,13 @@
     <t>Sales Forecast</t>
   </si>
   <si>
-    <t>Trend (CAGR)</t>
-  </si>
-  <si>
-    <t>Trend (Reg)</t>
-  </si>
-  <si>
     <t>Sales Method</t>
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>Trend</t>
   </si>
 </sst>
 </file>
@@ -162,10 +161,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1850,7 +1849,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="5153025" y="1885950"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:ext cx="4962525" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2183,7 +2182,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,78 +2206,78 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2289,14 +2288,14 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>5</v>
@@ -2305,10 +2304,10 @@
         <v>6</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>5</v>
@@ -2317,10 +2316,10 @@
         <v>6</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>5</v>
@@ -2329,10 +2328,10 @@
         <v>6</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V4" s="6" t="s">
         <v>5</v>
@@ -2354,14 +2353,14 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>5</v>
@@ -2394,16 +2393,16 @@
         <v>6</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -2583,7 +2582,7 @@
         <v>0.62</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:H8" si="8">C7/C6</f>
+        <f t="shared" ref="C8:D8" si="8">C7/C6</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="D8" s="2">

</xml_diff>